<commit_message>
added larvae PR data
</commit_message>
<xml_diff>
--- a/data/isotopes/sample_metadata_isotopes.xlsx
+++ b/data/isotopes/sample_metadata_isotopes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/isotopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08588095-64EE-3242-9970-27783376C654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0251644-746E-1B4A-8396-02BAD3E2AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="760" windowWidth="22140" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="134">
   <si>
     <t>sample_id</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>control run, from extra corals; each coral was a different colony</t>
+  </si>
+  <si>
+    <t>Molecular -40C mesh bag (2 bags total)</t>
   </si>
 </sst>
 </file>
@@ -812,8 +815,8 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1641,7 +1644,7 @@
         <v>116</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H31" t="s">
         <v>117</v>
@@ -1667,7 +1670,7 @@
         <v>116</v>
       </c>
       <c r="G32" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H32" t="s">
         <v>117</v>
@@ -1693,7 +1696,7 @@
         <v>116</v>
       </c>
       <c r="G33" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H33" t="s">
         <v>117</v>
@@ -1719,7 +1722,7 @@
         <v>116</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H34" t="s">
         <v>117</v>
@@ -1745,7 +1748,7 @@
         <v>116</v>
       </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H35" t="s">
         <v>117</v>
@@ -1771,7 +1774,7 @@
         <v>116</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H36" t="s">
         <v>117</v>
@@ -1797,7 +1800,7 @@
         <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H37" t="s">
         <v>117</v>
@@ -1823,7 +1826,7 @@
         <v>116</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H38" t="s">
         <v>117</v>
@@ -1849,7 +1852,7 @@
         <v>116</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H39" t="s">
         <v>117</v>
@@ -1875,7 +1878,7 @@
         <v>116</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H40" t="s">
         <v>117</v>
@@ -1901,7 +1904,7 @@
         <v>116</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H41" t="s">
         <v>117</v>
@@ -1927,7 +1930,7 @@
         <v>116</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H42" t="s">
         <v>117</v>
@@ -1982,7 +1985,7 @@
         <v>116</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H44" t="s">
         <v>117</v>
@@ -2008,7 +2011,7 @@
         <v>116</v>
       </c>
       <c r="G45" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H45" t="s">
         <v>117</v>
@@ -2034,7 +2037,7 @@
         <v>116</v>
       </c>
       <c r="G46" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H46" t="s">
         <v>117</v>
@@ -2089,7 +2092,7 @@
         <v>116</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H48" t="s">
         <v>117</v>
@@ -2118,7 +2121,7 @@
         <v>116</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H49" t="s">
         <v>117</v>
@@ -2144,7 +2147,7 @@
         <v>116</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H50" t="s">
         <v>117</v>
@@ -2170,7 +2173,7 @@
         <v>116</v>
       </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H51" t="s">
         <v>117</v>
@@ -2196,7 +2199,7 @@
         <v>116</v>
       </c>
       <c r="G52" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H52" t="s">
         <v>117</v>
@@ -2225,7 +2228,7 @@
         <v>116</v>
       </c>
       <c r="G53" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H53" t="s">
         <v>117</v>
@@ -2251,7 +2254,7 @@
         <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H54" t="s">
         <v>117</v>
@@ -2306,7 +2309,7 @@
         <v>116</v>
       </c>
       <c r="G56" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H56" t="s">
         <v>117</v>
@@ -2361,7 +2364,7 @@
         <v>116</v>
       </c>
       <c r="G58" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H58" t="s">
         <v>117</v>
@@ -2387,7 +2390,7 @@
         <v>116</v>
       </c>
       <c r="G59" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H59" t="s">
         <v>117</v>
@@ -2413,7 +2416,7 @@
         <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H60" t="s">
         <v>117</v>
@@ -2439,7 +2442,7 @@
         <v>116</v>
       </c>
       <c r="G61" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H61" t="s">
         <v>117</v>
@@ -2465,7 +2468,7 @@
         <v>116</v>
       </c>
       <c r="G62" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H62" t="s">
         <v>117</v>
@@ -2491,7 +2494,7 @@
         <v>116</v>
       </c>
       <c r="G63" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H63" t="s">
         <v>117</v>
@@ -2517,7 +2520,7 @@
         <v>116</v>
       </c>
       <c r="G64" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H64" t="s">
         <v>117</v>
@@ -2543,7 +2546,7 @@
         <v>116</v>
       </c>
       <c r="G65" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H65" t="s">
         <v>117</v>
@@ -2569,7 +2572,7 @@
         <v>116</v>
       </c>
       <c r="G66" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H66" t="s">
         <v>117</v>
@@ -2595,7 +2598,7 @@
         <v>116</v>
       </c>
       <c r="G67" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H67" t="s">
         <v>117</v>
@@ -2621,7 +2624,7 @@
         <v>116</v>
       </c>
       <c r="G68" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H68" t="s">
         <v>117</v>
@@ -2647,7 +2650,7 @@
         <v>116</v>
       </c>
       <c r="G69" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H69" t="s">
         <v>117</v>
@@ -2673,7 +2676,7 @@
         <v>116</v>
       </c>
       <c r="G70" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H70" t="s">
         <v>117</v>
@@ -2699,7 +2702,7 @@
         <v>116</v>
       </c>
       <c r="G71" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H71" t="s">
         <v>117</v>
@@ -2725,7 +2728,7 @@
         <v>116</v>
       </c>
       <c r="G72" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H72" t="s">
         <v>117</v>
@@ -2751,7 +2754,7 @@
         <v>116</v>
       </c>
       <c r="G73" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H73" t="s">
         <v>117</v>
@@ -2777,7 +2780,7 @@
         <v>116</v>
       </c>
       <c r="G74" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H74" t="s">
         <v>117</v>
@@ -2832,7 +2835,7 @@
         <v>116</v>
       </c>
       <c r="G76" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H76" t="s">
         <v>117</v>
@@ -2858,7 +2861,7 @@
         <v>116</v>
       </c>
       <c r="G77" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H77" t="s">
         <v>117</v>
@@ -2884,7 +2887,7 @@
         <v>116</v>
       </c>
       <c r="G78" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H78" t="s">
         <v>117</v>
@@ -2910,7 +2913,7 @@
         <v>116</v>
       </c>
       <c r="G79" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H79" t="s">
         <v>117</v>
@@ -2965,7 +2968,7 @@
         <v>116</v>
       </c>
       <c r="G81" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H81" t="s">
         <v>117</v>
@@ -2991,7 +2994,7 @@
         <v>116</v>
       </c>
       <c r="G82" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H82" t="s">
         <v>117</v>
@@ -3017,7 +3020,7 @@
         <v>116</v>
       </c>
       <c r="G83" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H83" t="s">
         <v>117</v>
@@ -3043,7 +3046,7 @@
         <v>116</v>
       </c>
       <c r="G84" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H84" t="s">
         <v>117</v>
@@ -3069,7 +3072,7 @@
         <v>116</v>
       </c>
       <c r="G85" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H85" t="s">
         <v>117</v>
@@ -3095,7 +3098,7 @@
         <v>116</v>
       </c>
       <c r="G86" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H86" t="s">
         <v>117</v>
@@ -3121,7 +3124,7 @@
         <v>116</v>
       </c>
       <c r="G87" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H87" t="s">
         <v>117</v>
@@ -3147,7 +3150,7 @@
         <v>116</v>
       </c>
       <c r="G88" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H88" t="s">
         <v>117</v>
@@ -3173,7 +3176,7 @@
         <v>116</v>
       </c>
       <c r="G89" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H89" t="s">
         <v>117</v>
@@ -3199,7 +3202,7 @@
         <v>116</v>
       </c>
       <c r="G90" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H90" t="s">
         <v>117</v>
@@ -3225,7 +3228,7 @@
         <v>116</v>
       </c>
       <c r="G91" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H91" t="s">
         <v>117</v>
@@ -3251,7 +3254,7 @@
         <v>116</v>
       </c>
       <c r="G92" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H92" t="s">
         <v>117</v>
@@ -3277,7 +3280,7 @@
         <v>116</v>
       </c>
       <c r="G93" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H93" t="s">
         <v>117</v>
@@ -3303,7 +3306,7 @@
         <v>116</v>
       </c>
       <c r="G94" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H94" t="s">
         <v>117</v>
@@ -3329,7 +3332,7 @@
         <v>116</v>
       </c>
       <c r="G95" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H95" t="s">
         <v>117</v>
@@ -3355,7 +3358,7 @@
         <v>116</v>
       </c>
       <c r="G96" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H96" t="s">
         <v>117</v>
@@ -3381,7 +3384,7 @@
         <v>116</v>
       </c>
       <c r="G97" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H97" t="s">
         <v>117</v>
@@ -3407,7 +3410,7 @@
         <v>116</v>
       </c>
       <c r="G98" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H98" t="s">
         <v>117</v>
@@ -3462,7 +3465,7 @@
         <v>116</v>
       </c>
       <c r="G100" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H100" t="s">
         <v>117</v>
@@ -3488,7 +3491,7 @@
         <v>116</v>
       </c>
       <c r="G101" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H101" t="s">
         <v>117</v>
@@ -3514,7 +3517,7 @@
         <v>116</v>
       </c>
       <c r="G102" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H102" t="s">
         <v>117</v>
@@ -3540,7 +3543,7 @@
         <v>116</v>
       </c>
       <c r="G103" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H103" t="s">
         <v>117</v>
@@ -3566,7 +3569,7 @@
         <v>116</v>
       </c>
       <c r="G104" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H104" t="s">
         <v>117</v>
@@ -3621,7 +3624,7 @@
         <v>116</v>
       </c>
       <c r="G106" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H106" t="s">
         <v>117</v>
@@ -3647,7 +3650,7 @@
         <v>116</v>
       </c>
       <c r="G107" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H107" t="s">
         <v>117</v>
@@ -3673,7 +3676,7 @@
         <v>116</v>
       </c>
       <c r="G108" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H108" t="s">
         <v>117</v>
@@ -3699,7 +3702,7 @@
         <v>116</v>
       </c>
       <c r="G109" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H109" t="s">
         <v>117</v>
@@ -3725,7 +3728,7 @@
         <v>116</v>
       </c>
       <c r="G110" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H110" t="s">
         <v>117</v>
@@ -3754,7 +3757,7 @@
         <v>116</v>
       </c>
       <c r="G111" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H111" t="s">
         <v>117</v>
@@ -3783,7 +3786,7 @@
         <v>116</v>
       </c>
       <c r="G112" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H112" t="s">
         <v>117</v>
@@ -3812,7 +3815,7 @@
         <v>116</v>
       </c>
       <c r="G113" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H113" t="s">
         <v>117</v>
@@ -3841,7 +3844,7 @@
         <v>116</v>
       </c>
       <c r="G114" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H114" t="s">
         <v>117</v>
@@ -3870,7 +3873,7 @@
         <v>116</v>
       </c>
       <c r="G115" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H115" t="s">
         <v>117</v>

</xml_diff>